<commit_message>
Clean up Decomposition directory: remove obsolete files, update README, and streamline structure
</commit_message>
<xml_diff>
--- a/stream3_visualization/Decomposition/data/2025-08-13_CH scenarios data_Decomposition_Compiled.xlsx
+++ b/stream3_visualization/Decomposition/data/2025-08-13_CH scenarios data_Decomposition_Compiled.xlsx
@@ -4,8 +4,9 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="All Sectors" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Buildings -Services" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="PassLandTransport" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="Feuille 1" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Buildings -Services" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="PassLandTransport" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_AtRisk_SimSetting_AutomaticallyGenerateReports">FALSE</definedName>
@@ -201,14 +202,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="tjr49sLGwscXTJ0opxRdW/9NZPwnDa144pZ9Kq9afBc="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataChecksum="uTIipyysWRvo2MbkOKX5F8cla+I1ZgKqRHJYfjYWRtA="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="27">
   <si>
     <t>Geography</t>
   </si>
@@ -240,7 +241,7 @@
     <t>Switzerland</t>
   </si>
   <si>
-    <t>Buildings-Residential</t>
+    <t>Buildings - Residential</t>
   </si>
   <si>
     <t>Scenario Basis</t>
@@ -258,13 +259,25 @@
     <t>Scenario Zer0 C</t>
   </si>
   <si>
-    <t>Buildings -Services</t>
+    <t>Buildings - Services</t>
   </si>
   <si>
-    <t>PassLandTransport</t>
+    <t>Passenger Land Transport</t>
   </si>
   <si>
     <t>Passenger Transport (Tpkm)</t>
+  </si>
+  <si>
+    <t>Industry - Cement</t>
+  </si>
+  <si>
+    <t>Production (Million of tons)</t>
+  </si>
+  <si>
+    <t>Cement industry</t>
+  </si>
+  <si>
+    <t>Steel industry</t>
   </si>
   <si>
     <t>Final Energy (Million toe)</t>
@@ -288,7 +301,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.000"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="8">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -313,6 +326,20 @@
     </font>
     <font>
       <b/>
+      <sz val="11.0"/>
+      <color rgb="FF222222"/>
+      <name val="&quot;Google Sans&quot;"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="&quot;Aptos Narrow&quot;"/>
+    </font>
+    <font>
       <sz val="11.0"/>
       <color rgb="FF222222"/>
       <name val="&quot;Google Sans&quot;"/>
@@ -350,7 +377,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -369,6 +396,15 @@
     <xf borderId="1" fillId="2" fontId="2" numFmtId="2" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyFont="1" applyNumberFormat="1"/>
@@ -390,6 +426,10 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -597,7 +637,10 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="4" width="11.75"/>
+    <col customWidth="1" min="1" max="1" width="11.75"/>
+    <col customWidth="1" min="2" max="2" width="20.13"/>
+    <col customWidth="1" min="3" max="3" width="29.5"/>
+    <col customWidth="1" min="4" max="4" width="11.75"/>
     <col customWidth="1" min="5" max="5" width="16.63"/>
     <col customWidth="1" min="6" max="6" width="18.88"/>
     <col customWidth="1" min="7" max="8" width="21.25"/>
@@ -4618,267 +4661,2643 @@
       <c r="J133" s="4"/>
     </row>
     <row r="134" ht="14.25" customHeight="1">
+      <c r="A134" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B134" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D134" s="2">
+        <v>2000.0</v>
+      </c>
+      <c r="E134" s="11">
+        <v>7.1842</v>
+      </c>
+      <c r="F134" s="11">
+        <v>4.840858641</v>
+      </c>
+      <c r="G134" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H134" s="11">
+        <v>3.84</v>
+      </c>
+      <c r="I134" s="11">
+        <v>10.1893</v>
+      </c>
       <c r="J134" s="4"/>
     </row>
     <row r="135" ht="14.25" customHeight="1">
+      <c r="A135" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B135" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C135" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D135" s="2">
+        <v>2005.0</v>
+      </c>
+      <c r="E135" s="11">
+        <v>7.4371</v>
+      </c>
+      <c r="F135" s="11">
+        <v>3.778461875</v>
+      </c>
+      <c r="G135" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H135" s="11">
+        <v>3.99</v>
+      </c>
+      <c r="I135" s="11">
+        <v>10.903</v>
+      </c>
       <c r="J135" s="4"/>
     </row>
     <row r="136" ht="14.25" customHeight="1">
+      <c r="A136" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B136" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D136" s="2">
+        <v>2010.0</v>
+      </c>
+      <c r="E136" s="11">
+        <v>7.827903</v>
+      </c>
+      <c r="F136" s="11">
+        <v>3.55141359</v>
+      </c>
+      <c r="G136" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H136" s="11">
+        <v>4.03</v>
+      </c>
+      <c r="I136" s="11">
+        <v>10.6873</v>
+      </c>
       <c r="J136" s="4"/>
     </row>
     <row r="137" ht="14.25" customHeight="1">
+      <c r="A137" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B137" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C137" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D137" s="2">
+        <v>2015.0</v>
+      </c>
+      <c r="E137" s="11">
+        <v>8.282396</v>
+      </c>
+      <c r="F137" s="11">
+        <v>3.912798776</v>
+      </c>
+      <c r="G137" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H137" s="11">
+        <v>3.7</v>
+      </c>
+      <c r="I137" s="11">
+        <v>9.79218</v>
+      </c>
       <c r="J137" s="4"/>
     </row>
     <row r="138" ht="14.25" customHeight="1">
+      <c r="A138" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B138" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D138" s="2">
+        <v>2020.0</v>
+      </c>
+      <c r="E138" s="11">
+        <v>8.705042598</v>
+      </c>
+      <c r="F138" s="11">
+        <v>4.307295172</v>
+      </c>
+      <c r="G138" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H138" s="11">
+        <v>3.56</v>
+      </c>
+      <c r="I138" s="11">
+        <v>9.40937</v>
+      </c>
       <c r="J138" s="4"/>
     </row>
     <row r="139" ht="14.25" customHeight="1">
+      <c r="A139" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B139" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C139" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D139" s="2">
+        <v>2025.0</v>
+      </c>
+      <c r="E139" s="11">
+        <v>9.107877966</v>
+      </c>
+      <c r="F139" s="11">
+        <v>3.974251411</v>
+      </c>
+      <c r="G139" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H139" s="11">
+        <v>3.33</v>
+      </c>
+      <c r="I139" s="11">
+        <v>7.98523</v>
+      </c>
       <c r="J139" s="4"/>
     </row>
     <row r="140" ht="14.25" customHeight="1">
+      <c r="A140" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B140" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C140" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D140" s="2">
+        <v>2030.0</v>
+      </c>
+      <c r="E140" s="11">
+        <v>9.491544346</v>
+      </c>
+      <c r="F140" s="11">
+        <v>4.1746495</v>
+      </c>
+      <c r="G140" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H140" s="11">
+        <v>3.12</v>
+      </c>
+      <c r="I140" s="11">
+        <v>6.97402</v>
+      </c>
       <c r="J140" s="4"/>
     </row>
     <row r="141" ht="14.25" customHeight="1">
+      <c r="A141" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B141" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D141" s="2">
+        <v>2035.0</v>
+      </c>
+      <c r="E141" s="11">
+        <v>9.81737221</v>
+      </c>
+      <c r="F141" s="11">
+        <v>4.1746495</v>
+      </c>
+      <c r="G141" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H141" s="11">
+        <v>2.94</v>
+      </c>
+      <c r="I141" s="11">
+        <v>5.97779</v>
+      </c>
       <c r="J141" s="4"/>
     </row>
     <row r="142" ht="14.25" customHeight="1">
+      <c r="A142" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B142" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D142" s="2">
+        <v>2040.0</v>
+      </c>
+      <c r="E142" s="11">
+        <v>10.01556327</v>
+      </c>
+      <c r="F142" s="11">
+        <v>4.1746495</v>
+      </c>
+      <c r="G142" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H142" s="11">
+        <v>2.77</v>
+      </c>
+      <c r="I142" s="11">
+        <v>4.67865</v>
+      </c>
       <c r="J142" s="4"/>
     </row>
     <row r="143" ht="14.25" customHeight="1">
+      <c r="A143" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B143" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D143" s="2">
+        <v>2045.0</v>
+      </c>
+      <c r="E143" s="11">
+        <v>10.15036585</v>
+      </c>
+      <c r="F143" s="11">
+        <v>4.1746495</v>
+      </c>
+      <c r="G143" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H143" s="11">
+        <v>2.63</v>
+      </c>
+      <c r="I143" s="11">
+        <v>2.121</v>
+      </c>
       <c r="J143" s="4"/>
     </row>
     <row r="144" ht="14.25" customHeight="1">
+      <c r="A144" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B144" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D144" s="2">
+        <v>2050.0</v>
+      </c>
+      <c r="E144" s="11">
+        <v>10.25697219</v>
+      </c>
+      <c r="F144" s="11">
+        <v>4.1746495</v>
+      </c>
+      <c r="G144" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H144" s="11">
+        <v>2.49</v>
+      </c>
+      <c r="I144" s="11">
+        <v>0.6134</v>
+      </c>
       <c r="J144" s="4"/>
     </row>
     <row r="145" ht="14.25" customHeight="1">
+      <c r="A145" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B145" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C145" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D145" s="2">
+        <v>2000.0</v>
+      </c>
+      <c r="E145" s="11">
+        <v>7.1842</v>
+      </c>
+      <c r="F145" s="11">
+        <v>4.840858641</v>
+      </c>
+      <c r="G145" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H145" s="11">
+        <v>3.84</v>
+      </c>
+      <c r="I145" s="11">
+        <v>10.1893</v>
+      </c>
       <c r="J145" s="4"/>
     </row>
     <row r="146" ht="14.25" customHeight="1">
+      <c r="A146" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B146" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C146" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D146" s="2">
+        <v>2005.0</v>
+      </c>
+      <c r="E146" s="11">
+        <v>7.4371</v>
+      </c>
+      <c r="F146" s="11">
+        <v>3.778461875</v>
+      </c>
+      <c r="G146" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H146" s="11">
+        <v>3.99</v>
+      </c>
+      <c r="I146" s="11">
+        <v>10.903</v>
+      </c>
       <c r="J146" s="4"/>
     </row>
     <row r="147" ht="14.25" customHeight="1">
+      <c r="A147" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B147" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C147" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D147" s="2">
+        <v>2010.0</v>
+      </c>
+      <c r="E147" s="11">
+        <v>7.827903</v>
+      </c>
+      <c r="F147" s="11">
+        <v>3.55141359</v>
+      </c>
+      <c r="G147" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H147" s="11">
+        <v>4.03</v>
+      </c>
+      <c r="I147" s="11">
+        <v>10.6873</v>
+      </c>
       <c r="J147" s="4"/>
     </row>
     <row r="148" ht="14.25" customHeight="1">
+      <c r="A148" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B148" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C148" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D148" s="2">
+        <v>2015.0</v>
+      </c>
+      <c r="E148" s="11">
+        <v>8.282396</v>
+      </c>
+      <c r="F148" s="11">
+        <v>3.912798776</v>
+      </c>
+      <c r="G148" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H148" s="11">
+        <v>3.7</v>
+      </c>
+      <c r="I148" s="11">
+        <v>9.79218</v>
+      </c>
       <c r="J148" s="4"/>
     </row>
     <row r="149" ht="14.25" customHeight="1">
+      <c r="A149" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B149" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C149" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D149" s="2">
+        <v>2020.0</v>
+      </c>
+      <c r="E149" s="11">
+        <v>8.705042598</v>
+      </c>
+      <c r="F149" s="11">
+        <v>4.307295172</v>
+      </c>
+      <c r="G149" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H149" s="11">
+        <v>3.58</v>
+      </c>
+      <c r="I149" s="11">
+        <v>9.43433</v>
+      </c>
       <c r="J149" s="4"/>
     </row>
     <row r="150" ht="14.25" customHeight="1">
+      <c r="A150" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B150" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D150" s="2">
+        <v>2025.0</v>
+      </c>
+      <c r="E150" s="11">
+        <v>9.107877966</v>
+      </c>
+      <c r="F150" s="11">
+        <v>3.974251411</v>
+      </c>
+      <c r="G150" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H150" s="11">
+        <v>3.35</v>
+      </c>
+      <c r="I150" s="11">
+        <v>8.01822</v>
+      </c>
       <c r="J150" s="4"/>
     </row>
     <row r="151" ht="14.25" customHeight="1">
+      <c r="A151" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B151" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C151" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D151" s="2">
+        <v>2030.0</v>
+      </c>
+      <c r="E151" s="11">
+        <v>9.491544346</v>
+      </c>
+      <c r="F151" s="11">
+        <v>4.1746495</v>
+      </c>
+      <c r="G151" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H151" s="11">
+        <v>3.14</v>
+      </c>
+      <c r="I151" s="11">
+        <v>7.05133</v>
+      </c>
       <c r="J151" s="4"/>
     </row>
     <row r="152" ht="14.25" customHeight="1">
+      <c r="A152" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B152" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C152" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D152" s="2">
+        <v>2035.0</v>
+      </c>
+      <c r="E152" s="11">
+        <v>9.81737221</v>
+      </c>
+      <c r="F152" s="11">
+        <v>4.1746495</v>
+      </c>
+      <c r="G152" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H152" s="11">
+        <v>2.96</v>
+      </c>
+      <c r="I152" s="11">
+        <v>6.10689</v>
+      </c>
       <c r="J152" s="4"/>
     </row>
     <row r="153" ht="14.25" customHeight="1">
+      <c r="A153" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B153" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C153" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D153" s="2">
+        <v>2040.0</v>
+      </c>
+      <c r="E153" s="11">
+        <v>10.01556327</v>
+      </c>
+      <c r="F153" s="11">
+        <v>4.1746495</v>
+      </c>
+      <c r="G153" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H153" s="11">
+        <v>2.79</v>
+      </c>
+      <c r="I153" s="11">
+        <v>4.79004</v>
+      </c>
       <c r="J153" s="4"/>
     </row>
     <row r="154" ht="14.25" customHeight="1">
+      <c r="A154" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B154" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C154" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D154" s="2">
+        <v>2045.0</v>
+      </c>
+      <c r="E154" s="11">
+        <v>10.15036585</v>
+      </c>
+      <c r="F154" s="11">
+        <v>4.1746495</v>
+      </c>
+      <c r="G154" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H154" s="11">
+        <v>2.65</v>
+      </c>
+      <c r="I154" s="11">
+        <v>2.13656</v>
+      </c>
       <c r="J154" s="4"/>
     </row>
     <row r="155" ht="14.25" customHeight="1">
+      <c r="A155" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B155" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D155" s="2">
+        <v>2050.0</v>
+      </c>
+      <c r="E155" s="11">
+        <v>10.25697219</v>
+      </c>
+      <c r="F155" s="11">
+        <v>4.1746495</v>
+      </c>
+      <c r="G155" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H155" s="11">
+        <v>2.51</v>
+      </c>
+      <c r="I155" s="11">
+        <v>0.5943</v>
+      </c>
       <c r="J155" s="4"/>
     </row>
     <row r="156" ht="14.25" customHeight="1">
+      <c r="A156" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B156" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C156" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D156" s="2">
+        <v>2000.0</v>
+      </c>
+      <c r="E156" s="11">
+        <v>7.1842</v>
+      </c>
+      <c r="F156" s="11">
+        <v>4.840858641</v>
+      </c>
+      <c r="G156" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H156" s="11">
+        <v>3.84</v>
+      </c>
+      <c r="I156" s="11">
+        <v>10.1893</v>
+      </c>
       <c r="J156" s="4"/>
     </row>
     <row r="157" ht="14.25" customHeight="1">
+      <c r="A157" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B157" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C157" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D157" s="2">
+        <v>2005.0</v>
+      </c>
+      <c r="E157" s="11">
+        <v>7.4371</v>
+      </c>
+      <c r="F157" s="11">
+        <v>3.778461875</v>
+      </c>
+      <c r="G157" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H157" s="11">
+        <v>3.99</v>
+      </c>
+      <c r="I157" s="11">
+        <v>10.903</v>
+      </c>
       <c r="J157" s="4"/>
     </row>
     <row r="158" ht="14.25" customHeight="1">
+      <c r="A158" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B158" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C158" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D158" s="2">
+        <v>2010.0</v>
+      </c>
+      <c r="E158" s="11">
+        <v>7.827903</v>
+      </c>
+      <c r="F158" s="11">
+        <v>3.55141359</v>
+      </c>
+      <c r="G158" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H158" s="11">
+        <v>4.03</v>
+      </c>
+      <c r="I158" s="11">
+        <v>10.6873</v>
+      </c>
       <c r="J158" s="4"/>
     </row>
     <row r="159" ht="14.25" customHeight="1">
+      <c r="A159" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B159" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C159" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D159" s="2">
+        <v>2015.0</v>
+      </c>
+      <c r="E159" s="11">
+        <v>8.282396</v>
+      </c>
+      <c r="F159" s="11">
+        <v>3.912798776</v>
+      </c>
+      <c r="G159" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H159" s="11">
+        <v>3.7</v>
+      </c>
+      <c r="I159" s="11">
+        <v>9.79218</v>
+      </c>
       <c r="J159" s="4"/>
     </row>
     <row r="160" ht="14.25" customHeight="1">
+      <c r="A160" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B160" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C160" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D160" s="2">
+        <v>2020.0</v>
+      </c>
+      <c r="E160" s="11">
+        <v>8.705042598</v>
+      </c>
+      <c r="F160" s="11">
+        <v>4.307295172</v>
+      </c>
+      <c r="G160" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H160" s="11">
+        <v>3.58</v>
+      </c>
+      <c r="I160" s="11">
+        <v>9.4292</v>
+      </c>
       <c r="J160" s="4"/>
     </row>
     <row r="161" ht="14.25" customHeight="1">
+      <c r="A161" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B161" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C161" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D161" s="2">
+        <v>2025.0</v>
+      </c>
+      <c r="E161" s="11">
+        <v>9.107877966</v>
+      </c>
+      <c r="F161" s="11">
+        <v>3.974251411</v>
+      </c>
+      <c r="G161" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H161" s="11">
+        <v>3.35</v>
+      </c>
+      <c r="I161" s="11">
+        <v>8.00421</v>
+      </c>
       <c r="J161" s="4"/>
     </row>
     <row r="162" ht="14.25" customHeight="1">
+      <c r="A162" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B162" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C162" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D162" s="2">
+        <v>2030.0</v>
+      </c>
+      <c r="E162" s="11">
+        <v>9.491544346</v>
+      </c>
+      <c r="F162" s="11">
+        <v>4.1746495</v>
+      </c>
+      <c r="G162" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H162" s="11">
+        <v>3.15</v>
+      </c>
+      <c r="I162" s="11">
+        <v>7.03097</v>
+      </c>
       <c r="J162" s="4"/>
     </row>
     <row r="163" ht="14.25" customHeight="1">
+      <c r="A163" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B163" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C163" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D163" s="2">
+        <v>2035.0</v>
+      </c>
+      <c r="E163" s="11">
+        <v>9.81737221</v>
+      </c>
+      <c r="F163" s="11">
+        <v>4.1746495</v>
+      </c>
+      <c r="G163" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H163" s="11">
+        <v>2.97</v>
+      </c>
+      <c r="I163" s="11">
+        <v>6.15414</v>
+      </c>
       <c r="J163" s="4"/>
     </row>
     <row r="164" ht="14.25" customHeight="1">
+      <c r="A164" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B164" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C164" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D164" s="2">
+        <v>2040.0</v>
+      </c>
+      <c r="E164" s="11">
+        <v>10.01556327</v>
+      </c>
+      <c r="F164" s="11">
+        <v>4.1746495</v>
+      </c>
+      <c r="G164" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H164" s="11">
+        <v>2.8</v>
+      </c>
+      <c r="I164" s="11">
+        <v>4.92137</v>
+      </c>
       <c r="J164" s="4"/>
     </row>
     <row r="165" ht="14.25" customHeight="1">
+      <c r="A165" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B165" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C165" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D165" s="2">
+        <v>2045.0</v>
+      </c>
+      <c r="E165" s="11">
+        <v>10.15036585</v>
+      </c>
+      <c r="F165" s="11">
+        <v>4.1746495</v>
+      </c>
+      <c r="G165" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H165" s="11">
+        <v>2.66</v>
+      </c>
+      <c r="I165" s="11">
+        <v>2.17641</v>
+      </c>
       <c r="J165" s="4"/>
     </row>
     <row r="166" ht="14.25" customHeight="1">
+      <c r="A166" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B166" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C166" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D166" s="2">
+        <v>2050.0</v>
+      </c>
+      <c r="E166" s="11">
+        <v>10.25697219</v>
+      </c>
+      <c r="F166" s="11">
+        <v>4.1746495</v>
+      </c>
+      <c r="G166" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H166" s="11">
+        <v>2.52</v>
+      </c>
+      <c r="I166" s="11">
+        <v>0.56564</v>
+      </c>
       <c r="J166" s="4"/>
     </row>
     <row r="167" ht="14.25" customHeight="1">
+      <c r="A167" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B167" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C167" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D167" s="2">
+        <v>2000.0</v>
+      </c>
+      <c r="E167" s="11">
+        <v>7.1842</v>
+      </c>
+      <c r="F167" s="11">
+        <v>4.840858641</v>
+      </c>
+      <c r="G167" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H167" s="11">
+        <v>3.84</v>
+      </c>
+      <c r="I167" s="11">
+        <v>10.1893</v>
+      </c>
       <c r="J167" s="4"/>
     </row>
     <row r="168" ht="14.25" customHeight="1">
+      <c r="A168" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B168" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C168" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D168" s="2">
+        <v>2005.0</v>
+      </c>
+      <c r="E168" s="11">
+        <v>7.4371</v>
+      </c>
+      <c r="F168" s="11">
+        <v>3.778461875</v>
+      </c>
+      <c r="G168" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H168" s="11">
+        <v>3.99</v>
+      </c>
+      <c r="I168" s="11">
+        <v>10.903</v>
+      </c>
       <c r="J168" s="4"/>
     </row>
     <row r="169" ht="14.25" customHeight="1">
+      <c r="A169" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B169" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C169" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D169" s="2">
+        <v>2010.0</v>
+      </c>
+      <c r="E169" s="11">
+        <v>7.827903</v>
+      </c>
+      <c r="F169" s="11">
+        <v>3.55141359</v>
+      </c>
+      <c r="G169" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H169" s="11">
+        <v>4.03</v>
+      </c>
+      <c r="I169" s="11">
+        <v>10.6873</v>
+      </c>
       <c r="J169" s="4"/>
     </row>
     <row r="170" ht="14.25" customHeight="1">
+      <c r="A170" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B170" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C170" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D170" s="2">
+        <v>2015.0</v>
+      </c>
+      <c r="E170" s="11">
+        <v>8.282396</v>
+      </c>
+      <c r="F170" s="11">
+        <v>3.912798776</v>
+      </c>
+      <c r="G170" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H170" s="11">
+        <v>3.7</v>
+      </c>
+      <c r="I170" s="11">
+        <v>9.79218</v>
+      </c>
       <c r="J170" s="4"/>
     </row>
     <row r="171" ht="14.25" customHeight="1">
+      <c r="A171" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B171" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C171" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D171" s="2">
+        <v>2020.0</v>
+      </c>
+      <c r="E171" s="11">
+        <v>8.705042598</v>
+      </c>
+      <c r="F171" s="11">
+        <v>4.307295172</v>
+      </c>
+      <c r="G171" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H171" s="11">
+        <v>3.58</v>
+      </c>
+      <c r="I171" s="11">
+        <v>9.42986</v>
+      </c>
       <c r="J171" s="4"/>
     </row>
     <row r="172" ht="14.25" customHeight="1">
+      <c r="A172" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B172" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C172" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D172" s="2">
+        <v>2025.0</v>
+      </c>
+      <c r="E172" s="11">
+        <v>9.107877966</v>
+      </c>
+      <c r="F172" s="11">
+        <v>3.974251411</v>
+      </c>
+      <c r="G172" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H172" s="11">
+        <v>3.35</v>
+      </c>
+      <c r="I172" s="11">
+        <v>8.01852</v>
+      </c>
       <c r="J172" s="4"/>
     </row>
     <row r="173" ht="14.25" customHeight="1">
+      <c r="A173" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B173" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C173" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D173" s="2">
+        <v>2030.0</v>
+      </c>
+      <c r="E173" s="11">
+        <v>9.491544346</v>
+      </c>
+      <c r="F173" s="11">
+        <v>4.1746495</v>
+      </c>
+      <c r="G173" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H173" s="11">
+        <v>3.15</v>
+      </c>
+      <c r="I173" s="11">
+        <v>7.03544</v>
+      </c>
       <c r="J173" s="4"/>
     </row>
     <row r="174" ht="14.25" customHeight="1">
+      <c r="A174" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B174" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C174" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D174" s="2">
+        <v>2035.0</v>
+      </c>
+      <c r="E174" s="11">
+        <v>9.81737221</v>
+      </c>
+      <c r="F174" s="11">
+        <v>4.1746495</v>
+      </c>
+      <c r="G174" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H174" s="11">
+        <v>2.97</v>
+      </c>
+      <c r="I174" s="11">
+        <v>6.03674</v>
+      </c>
       <c r="J174" s="4"/>
     </row>
     <row r="175" ht="14.25" customHeight="1">
+      <c r="A175" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B175" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C175" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D175" s="2">
+        <v>2040.0</v>
+      </c>
+      <c r="E175" s="11">
+        <v>10.01556327</v>
+      </c>
+      <c r="F175" s="11">
+        <v>4.1746495</v>
+      </c>
+      <c r="G175" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H175" s="11">
+        <v>2.8</v>
+      </c>
+      <c r="I175" s="11">
+        <v>4.6921</v>
+      </c>
       <c r="J175" s="4"/>
     </row>
     <row r="176" ht="14.25" customHeight="1">
+      <c r="A176" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B176" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C176" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D176" s="2">
+        <v>2045.0</v>
+      </c>
+      <c r="E176" s="11">
+        <v>10.15036585</v>
+      </c>
+      <c r="F176" s="11">
+        <v>4.1746495</v>
+      </c>
+      <c r="G176" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H176" s="11">
+        <v>2.66</v>
+      </c>
+      <c r="I176" s="11">
+        <v>2.08916</v>
+      </c>
       <c r="J176" s="4"/>
     </row>
     <row r="177" ht="14.25" customHeight="1">
+      <c r="A177" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B177" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C177" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D177" s="2">
+        <v>2050.0</v>
+      </c>
+      <c r="E177" s="11">
+        <v>10.25697219</v>
+      </c>
+      <c r="F177" s="11">
+        <v>4.1746495</v>
+      </c>
+      <c r="G177" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H177" s="11">
+        <v>2.52</v>
+      </c>
+      <c r="I177" s="11">
+        <v>0.55273</v>
+      </c>
       <c r="J177" s="4"/>
     </row>
     <row r="178" ht="14.25" customHeight="1">
+      <c r="A178" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B178" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C178" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D178" s="2">
+        <v>2000.0</v>
+      </c>
+      <c r="E178" s="11">
+        <v>7.1842</v>
+      </c>
+      <c r="F178" s="11">
+        <v>1.596232917</v>
+      </c>
+      <c r="G178" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H178" s="11">
+        <v>3.84</v>
+      </c>
+      <c r="I178" s="11">
+        <v>10.1893</v>
+      </c>
       <c r="J178" s="4"/>
     </row>
     <row r="179" ht="14.25" customHeight="1">
+      <c r="A179" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B179" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C179" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D179" s="2">
+        <v>2005.0</v>
+      </c>
+      <c r="E179" s="11">
+        <v>7.4371</v>
+      </c>
+      <c r="F179" s="11">
+        <v>1.056661227</v>
+      </c>
+      <c r="G179" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H179" s="11">
+        <v>3.99</v>
+      </c>
+      <c r="I179" s="11">
+        <v>10.903</v>
+      </c>
       <c r="J179" s="4"/>
     </row>
     <row r="180" ht="14.25" customHeight="1">
+      <c r="A180" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B180" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C180" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D180" s="2">
+        <v>2010.0</v>
+      </c>
+      <c r="E180" s="11">
+        <v>7.827903</v>
+      </c>
+      <c r="F180" s="11">
+        <v>1.26964373</v>
+      </c>
+      <c r="G180" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H180" s="11">
+        <v>4.03</v>
+      </c>
+      <c r="I180" s="11">
+        <v>10.6873</v>
+      </c>
       <c r="J180" s="4"/>
     </row>
     <row r="181" ht="14.25" customHeight="1">
+      <c r="A181" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B181" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C181" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D181" s="2">
+        <v>2015.0</v>
+      </c>
+      <c r="E181" s="11">
+        <v>8.282396</v>
+      </c>
+      <c r="F181" s="11">
+        <v>1.28875533</v>
+      </c>
+      <c r="G181" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H181" s="11">
+        <v>3.7</v>
+      </c>
+      <c r="I181" s="11">
+        <v>9.79218</v>
+      </c>
       <c r="J181" s="4"/>
     </row>
     <row r="182" ht="14.25" customHeight="1">
+      <c r="A182" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B182" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C182" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D182" s="2">
+        <v>2020.0</v>
+      </c>
+      <c r="E182" s="11">
+        <v>8.705042598</v>
+      </c>
+      <c r="F182" s="11">
+        <v>1.386954269</v>
+      </c>
+      <c r="G182" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H182" s="11">
+        <v>3.56</v>
+      </c>
+      <c r="I182" s="11">
+        <v>9.40937</v>
+      </c>
       <c r="J182" s="4"/>
     </row>
     <row r="183" ht="14.25" customHeight="1">
+      <c r="A183" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B183" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C183" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D183" s="2">
+        <v>2025.0</v>
+      </c>
+      <c r="E183" s="11">
+        <v>9.107877966</v>
+      </c>
+      <c r="F183" s="11">
+        <v>1.456298108</v>
+      </c>
+      <c r="G183" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H183" s="11">
+        <v>3.33</v>
+      </c>
+      <c r="I183" s="11">
+        <v>7.98523</v>
+      </c>
       <c r="J183" s="4"/>
     </row>
     <row r="184" ht="14.25" customHeight="1">
+      <c r="A184" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B184" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C184" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D184" s="2">
+        <v>2030.0</v>
+      </c>
+      <c r="E184" s="11">
+        <v>9.491544346</v>
+      </c>
+      <c r="F184" s="11">
+        <v>1.508811849</v>
+      </c>
+      <c r="G184" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H184" s="11">
+        <v>3.12</v>
+      </c>
+      <c r="I184" s="11">
+        <v>6.97402</v>
+      </c>
       <c r="J184" s="4"/>
     </row>
     <row r="185" ht="14.25" customHeight="1">
+      <c r="A185" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B185" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C185" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D185" s="2">
+        <v>2035.0</v>
+      </c>
+      <c r="E185" s="11">
+        <v>9.81737221</v>
+      </c>
+      <c r="F185" s="11">
+        <v>1.514126855</v>
+      </c>
+      <c r="G185" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H185" s="11">
+        <v>2.94</v>
+      </c>
+      <c r="I185" s="11">
+        <v>5.97779</v>
+      </c>
       <c r="J185" s="4"/>
     </row>
     <row r="186" ht="14.25" customHeight="1">
+      <c r="A186" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B186" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C186" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D186" s="2">
+        <v>2040.0</v>
+      </c>
+      <c r="E186" s="11">
+        <v>10.01556327</v>
+      </c>
+      <c r="F186" s="11">
+        <v>1.4989215</v>
+      </c>
+      <c r="G186" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H186" s="11">
+        <v>2.77</v>
+      </c>
+      <c r="I186" s="11">
+        <v>4.67865</v>
+      </c>
       <c r="J186" s="4"/>
     </row>
     <row r="187" ht="14.25" customHeight="1">
+      <c r="A187" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B187" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C187" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D187" s="2">
+        <v>2045.0</v>
+      </c>
+      <c r="E187" s="11">
+        <v>10.15036585</v>
+      </c>
+      <c r="F187" s="11">
+        <v>1.50163712</v>
+      </c>
+      <c r="G187" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H187" s="11">
+        <v>2.63</v>
+      </c>
+      <c r="I187" s="11">
+        <v>2.121</v>
+      </c>
       <c r="J187" s="4"/>
     </row>
     <row r="188" ht="14.25" customHeight="1">
+      <c r="A188" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B188" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C188" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D188" s="2">
+        <v>2050.0</v>
+      </c>
+      <c r="E188" s="11">
+        <v>10.25697219</v>
+      </c>
+      <c r="F188" s="11">
+        <v>1.511411236</v>
+      </c>
+      <c r="G188" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H188" s="11">
+        <v>2.49</v>
+      </c>
+      <c r="I188" s="11">
+        <v>0.6134</v>
+      </c>
       <c r="J188" s="4"/>
     </row>
     <row r="189" ht="14.25" customHeight="1">
+      <c r="A189" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B189" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C189" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D189" s="2">
+        <v>2000.0</v>
+      </c>
+      <c r="E189" s="11">
+        <v>7.1842</v>
+      </c>
+      <c r="F189" s="11">
+        <v>1.596232917</v>
+      </c>
+      <c r="G189" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H189" s="11">
+        <v>3.84</v>
+      </c>
+      <c r="I189" s="11">
+        <v>10.1893</v>
+      </c>
       <c r="J189" s="4"/>
     </row>
     <row r="190" ht="14.25" customHeight="1">
+      <c r="A190" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B190" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C190" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D190" s="2">
+        <v>2005.0</v>
+      </c>
+      <c r="E190" s="11">
+        <v>7.4371</v>
+      </c>
+      <c r="F190" s="11">
+        <v>1.056661227</v>
+      </c>
+      <c r="G190" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H190" s="11">
+        <v>3.99</v>
+      </c>
+      <c r="I190" s="11">
+        <v>10.903</v>
+      </c>
       <c r="J190" s="4"/>
     </row>
     <row r="191" ht="14.25" customHeight="1">
+      <c r="A191" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B191" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C191" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D191" s="2">
+        <v>2010.0</v>
+      </c>
+      <c r="E191" s="11">
+        <v>7.827903</v>
+      </c>
+      <c r="F191" s="11">
+        <v>1.26964373</v>
+      </c>
+      <c r="G191" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H191" s="11">
+        <v>4.03</v>
+      </c>
+      <c r="I191" s="11">
+        <v>10.6873</v>
+      </c>
       <c r="J191" s="4"/>
     </row>
     <row r="192" ht="14.25" customHeight="1">
+      <c r="A192" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B192" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C192" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D192" s="2">
+        <v>2015.0</v>
+      </c>
+      <c r="E192" s="11">
+        <v>8.282396</v>
+      </c>
+      <c r="F192" s="11">
+        <v>1.28875533</v>
+      </c>
+      <c r="G192" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H192" s="11">
+        <v>3.7</v>
+      </c>
+      <c r="I192" s="11">
+        <v>9.79218</v>
+      </c>
       <c r="J192" s="4"/>
     </row>
     <row r="193" ht="14.25" customHeight="1">
+      <c r="A193" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B193" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C193" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D193" s="2">
+        <v>2020.0</v>
+      </c>
+      <c r="E193" s="11">
+        <v>8.705042598</v>
+      </c>
+      <c r="F193" s="11">
+        <v>1.386954269</v>
+      </c>
+      <c r="G193" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H193" s="11">
+        <v>3.58</v>
+      </c>
+      <c r="I193" s="11">
+        <v>9.43433</v>
+      </c>
       <c r="J193" s="4"/>
     </row>
     <row r="194" ht="14.25" customHeight="1">
+      <c r="A194" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B194" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C194" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D194" s="2">
+        <v>2025.0</v>
+      </c>
+      <c r="E194" s="11">
+        <v>9.107877966</v>
+      </c>
+      <c r="F194" s="11">
+        <v>1.456298108</v>
+      </c>
+      <c r="G194" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H194" s="11">
+        <v>3.35</v>
+      </c>
+      <c r="I194" s="11">
+        <v>8.01822</v>
+      </c>
       <c r="J194" s="4"/>
     </row>
     <row r="195" ht="14.25" customHeight="1">
+      <c r="A195" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B195" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C195" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D195" s="2">
+        <v>2030.0</v>
+      </c>
+      <c r="E195" s="11">
+        <v>9.491544346</v>
+      </c>
+      <c r="F195" s="11">
+        <v>1.508811849</v>
+      </c>
+      <c r="G195" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H195" s="11">
+        <v>3.14</v>
+      </c>
+      <c r="I195" s="11">
+        <v>7.05133</v>
+      </c>
       <c r="J195" s="4"/>
     </row>
     <row r="196" ht="14.25" customHeight="1">
+      <c r="A196" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B196" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C196" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D196" s="2">
+        <v>2035.0</v>
+      </c>
+      <c r="E196" s="11">
+        <v>9.81737221</v>
+      </c>
+      <c r="F196" s="11">
+        <v>1.514126855</v>
+      </c>
+      <c r="G196" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H196" s="11">
+        <v>2.96</v>
+      </c>
+      <c r="I196" s="11">
+        <v>6.10689</v>
+      </c>
       <c r="J196" s="4"/>
     </row>
     <row r="197" ht="14.25" customHeight="1">
+      <c r="A197" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B197" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C197" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D197" s="2">
+        <v>2040.0</v>
+      </c>
+      <c r="E197" s="11">
+        <v>10.01556327</v>
+      </c>
+      <c r="F197" s="11">
+        <v>1.4989215</v>
+      </c>
+      <c r="G197" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H197" s="11">
+        <v>2.79</v>
+      </c>
+      <c r="I197" s="11">
+        <v>4.79004</v>
+      </c>
       <c r="J197" s="4"/>
     </row>
     <row r="198" ht="14.25" customHeight="1">
+      <c r="A198" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B198" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C198" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D198" s="2">
+        <v>2045.0</v>
+      </c>
+      <c r="E198" s="11">
+        <v>10.15036585</v>
+      </c>
+      <c r="F198" s="11">
+        <v>1.50163712</v>
+      </c>
+      <c r="G198" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H198" s="11">
+        <v>2.65</v>
+      </c>
+      <c r="I198" s="11">
+        <v>2.13656</v>
+      </c>
       <c r="J198" s="4"/>
     </row>
     <row r="199" ht="14.25" customHeight="1">
+      <c r="A199" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B199" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C199" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D199" s="2">
+        <v>2050.0</v>
+      </c>
+      <c r="E199" s="11">
+        <v>10.25697219</v>
+      </c>
+      <c r="F199" s="11">
+        <v>1.511411236</v>
+      </c>
+      <c r="G199" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H199" s="11">
+        <v>2.51</v>
+      </c>
+      <c r="I199" s="11">
+        <v>0.5943</v>
+      </c>
       <c r="J199" s="4"/>
     </row>
     <row r="200" ht="14.25" customHeight="1">
+      <c r="A200" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B200" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C200" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D200" s="2">
+        <v>2000.0</v>
+      </c>
+      <c r="E200" s="11">
+        <v>7.1842</v>
+      </c>
+      <c r="F200" s="11">
+        <v>1.596232917</v>
+      </c>
+      <c r="G200" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H200" s="11">
+        <v>3.84</v>
+      </c>
+      <c r="I200" s="11">
+        <v>10.1893</v>
+      </c>
       <c r="J200" s="4"/>
     </row>
     <row r="201" ht="14.25" customHeight="1">
+      <c r="A201" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B201" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C201" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D201" s="2">
+        <v>2005.0</v>
+      </c>
+      <c r="E201" s="11">
+        <v>7.4371</v>
+      </c>
+      <c r="F201" s="11">
+        <v>1.056661227</v>
+      </c>
+      <c r="G201" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H201" s="11">
+        <v>3.99</v>
+      </c>
+      <c r="I201" s="11">
+        <v>10.903</v>
+      </c>
       <c r="J201" s="4"/>
     </row>
     <row r="202" ht="14.25" customHeight="1">
+      <c r="A202" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B202" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C202" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D202" s="2">
+        <v>2010.0</v>
+      </c>
+      <c r="E202" s="11">
+        <v>7.827903</v>
+      </c>
+      <c r="F202" s="11">
+        <v>1.26964373</v>
+      </c>
+      <c r="G202" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H202" s="11">
+        <v>4.03</v>
+      </c>
+      <c r="I202" s="11">
+        <v>10.6873</v>
+      </c>
       <c r="J202" s="4"/>
     </row>
     <row r="203" ht="14.25" customHeight="1">
+      <c r="A203" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B203" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C203" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D203" s="2">
+        <v>2015.0</v>
+      </c>
+      <c r="E203" s="11">
+        <v>8.282396</v>
+      </c>
+      <c r="F203" s="11">
+        <v>1.28875533</v>
+      </c>
+      <c r="G203" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H203" s="11">
+        <v>3.7</v>
+      </c>
+      <c r="I203" s="11">
+        <v>9.79218</v>
+      </c>
       <c r="J203" s="4"/>
     </row>
     <row r="204" ht="14.25" customHeight="1">
+      <c r="A204" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B204" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C204" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D204" s="2">
+        <v>2020.0</v>
+      </c>
+      <c r="E204" s="11">
+        <v>8.705042598</v>
+      </c>
+      <c r="F204" s="11">
+        <v>1.386954269</v>
+      </c>
+      <c r="G204" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H204" s="11">
+        <v>3.58</v>
+      </c>
+      <c r="I204" s="11">
+        <v>9.4292</v>
+      </c>
       <c r="J204" s="4"/>
     </row>
     <row r="205" ht="14.25" customHeight="1">
+      <c r="A205" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B205" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C205" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D205" s="2">
+        <v>2025.0</v>
+      </c>
+      <c r="E205" s="11">
+        <v>9.107877966</v>
+      </c>
+      <c r="F205" s="11">
+        <v>1.456298108</v>
+      </c>
+      <c r="G205" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H205" s="11">
+        <v>3.35</v>
+      </c>
+      <c r="I205" s="11">
+        <v>8.00421</v>
+      </c>
       <c r="J205" s="4"/>
     </row>
     <row r="206" ht="14.25" customHeight="1">
+      <c r="A206" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B206" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C206" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D206" s="2">
+        <v>2030.0</v>
+      </c>
+      <c r="E206" s="11">
+        <v>9.491544346</v>
+      </c>
+      <c r="F206" s="11">
+        <v>1.508811849</v>
+      </c>
+      <c r="G206" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H206" s="11">
+        <v>3.15</v>
+      </c>
+      <c r="I206" s="11">
+        <v>7.03097</v>
+      </c>
       <c r="J206" s="4"/>
     </row>
     <row r="207" ht="14.25" customHeight="1">
+      <c r="A207" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B207" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C207" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D207" s="2">
+        <v>2035.0</v>
+      </c>
+      <c r="E207" s="11">
+        <v>9.81737221</v>
+      </c>
+      <c r="F207" s="11">
+        <v>1.514126855</v>
+      </c>
+      <c r="G207" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H207" s="11">
+        <v>2.97</v>
+      </c>
+      <c r="I207" s="11">
+        <v>6.15414</v>
+      </c>
       <c r="J207" s="4"/>
     </row>
     <row r="208" ht="14.25" customHeight="1">
+      <c r="A208" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B208" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C208" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D208" s="2">
+        <v>2040.0</v>
+      </c>
+      <c r="E208" s="11">
+        <v>10.01556327</v>
+      </c>
+      <c r="F208" s="11">
+        <v>1.4989215</v>
+      </c>
+      <c r="G208" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H208" s="11">
+        <v>2.8</v>
+      </c>
+      <c r="I208" s="11">
+        <v>4.92137</v>
+      </c>
       <c r="J208" s="4"/>
     </row>
     <row r="209" ht="14.25" customHeight="1">
+      <c r="A209" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B209" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C209" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D209" s="2">
+        <v>2045.0</v>
+      </c>
+      <c r="E209" s="11">
+        <v>10.15036585</v>
+      </c>
+      <c r="F209" s="11">
+        <v>1.50163712</v>
+      </c>
+      <c r="G209" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H209" s="11">
+        <v>2.66</v>
+      </c>
+      <c r="I209" s="11">
+        <v>2.17641</v>
+      </c>
       <c r="J209" s="4"/>
     </row>
     <row r="210" ht="14.25" customHeight="1">
+      <c r="A210" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B210" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C210" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D210" s="2">
+        <v>2050.0</v>
+      </c>
+      <c r="E210" s="11">
+        <v>10.25697219</v>
+      </c>
+      <c r="F210" s="11">
+        <v>1.511411236</v>
+      </c>
+      <c r="G210" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H210" s="11">
+        <v>2.52</v>
+      </c>
+      <c r="I210" s="11">
+        <v>0.56564</v>
+      </c>
       <c r="J210" s="4"/>
     </row>
     <row r="211" ht="14.25" customHeight="1">
+      <c r="A211" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B211" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C211" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D211" s="2">
+        <v>2000.0</v>
+      </c>
+      <c r="E211" s="11">
+        <v>7.1842</v>
+      </c>
+      <c r="F211" s="11">
+        <v>1.596232917</v>
+      </c>
+      <c r="G211" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H211" s="11">
+        <v>3.84</v>
+      </c>
+      <c r="I211" s="11">
+        <v>10.1893</v>
+      </c>
       <c r="J211" s="4"/>
     </row>
     <row r="212" ht="14.25" customHeight="1">
+      <c r="A212" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B212" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C212" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D212" s="2">
+        <v>2005.0</v>
+      </c>
+      <c r="E212" s="11">
+        <v>7.4371</v>
+      </c>
+      <c r="F212" s="11">
+        <v>1.056661227</v>
+      </c>
+      <c r="G212" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H212" s="11">
+        <v>3.99</v>
+      </c>
+      <c r="I212" s="11">
+        <v>10.903</v>
+      </c>
       <c r="J212" s="4"/>
     </row>
     <row r="213" ht="14.25" customHeight="1">
+      <c r="A213" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B213" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C213" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D213" s="2">
+        <v>2010.0</v>
+      </c>
+      <c r="E213" s="11">
+        <v>7.827903</v>
+      </c>
+      <c r="F213" s="11">
+        <v>1.26964373</v>
+      </c>
+      <c r="G213" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H213" s="11">
+        <v>4.03</v>
+      </c>
+      <c r="I213" s="11">
+        <v>10.6873</v>
+      </c>
       <c r="J213" s="4"/>
     </row>
     <row r="214" ht="14.25" customHeight="1">
+      <c r="A214" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B214" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C214" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D214" s="2">
+        <v>2015.0</v>
+      </c>
+      <c r="E214" s="11">
+        <v>8.282396</v>
+      </c>
+      <c r="F214" s="11">
+        <v>1.28875533</v>
+      </c>
+      <c r="G214" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H214" s="11">
+        <v>3.7</v>
+      </c>
+      <c r="I214" s="11">
+        <v>9.79218</v>
+      </c>
       <c r="J214" s="4"/>
     </row>
     <row r="215" ht="14.25" customHeight="1">
+      <c r="A215" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B215" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C215" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D215" s="2">
+        <v>2020.0</v>
+      </c>
+      <c r="E215" s="11">
+        <v>8.705042598</v>
+      </c>
+      <c r="F215" s="11">
+        <v>1.386954269</v>
+      </c>
+      <c r="G215" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H215" s="11">
+        <v>3.58</v>
+      </c>
+      <c r="I215" s="11">
+        <v>9.42986</v>
+      </c>
       <c r="J215" s="4"/>
     </row>
     <row r="216" ht="14.25" customHeight="1">
+      <c r="A216" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B216" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C216" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D216" s="2">
+        <v>2025.0</v>
+      </c>
+      <c r="E216" s="11">
+        <v>9.107877966</v>
+      </c>
+      <c r="F216" s="11">
+        <v>1.456298108</v>
+      </c>
+      <c r="G216" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H216" s="11">
+        <v>3.35</v>
+      </c>
+      <c r="I216" s="11">
+        <v>8.01852</v>
+      </c>
       <c r="J216" s="4"/>
     </row>
     <row r="217" ht="14.25" customHeight="1">
+      <c r="A217" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B217" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C217" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D217" s="2">
+        <v>2030.0</v>
+      </c>
+      <c r="E217" s="11">
+        <v>9.491544346</v>
+      </c>
+      <c r="F217" s="11">
+        <v>1.508811849</v>
+      </c>
+      <c r="G217" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H217" s="11">
+        <v>3.15</v>
+      </c>
+      <c r="I217" s="11">
+        <v>7.03544</v>
+      </c>
       <c r="J217" s="4"/>
     </row>
     <row r="218" ht="14.25" customHeight="1">
+      <c r="A218" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B218" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C218" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D218" s="2">
+        <v>2035.0</v>
+      </c>
+      <c r="E218" s="11">
+        <v>9.81737221</v>
+      </c>
+      <c r="F218" s="11">
+        <v>1.514126855</v>
+      </c>
+      <c r="G218" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H218" s="11">
+        <v>2.97</v>
+      </c>
+      <c r="I218" s="11">
+        <v>6.03674</v>
+      </c>
       <c r="J218" s="4"/>
     </row>
     <row r="219" ht="14.25" customHeight="1">
+      <c r="A219" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B219" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C219" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D219" s="2">
+        <v>2040.0</v>
+      </c>
+      <c r="E219" s="11">
+        <v>10.01556327</v>
+      </c>
+      <c r="F219" s="11">
+        <v>1.4989215</v>
+      </c>
+      <c r="G219" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H219" s="11">
+        <v>2.8</v>
+      </c>
+      <c r="I219" s="11">
+        <v>4.6921</v>
+      </c>
       <c r="J219" s="4"/>
     </row>
     <row r="220" ht="14.25" customHeight="1">
+      <c r="A220" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B220" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C220" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D220" s="2">
+        <v>2045.0</v>
+      </c>
+      <c r="E220" s="11">
+        <v>10.15036585</v>
+      </c>
+      <c r="F220" s="11">
+        <v>1.50163712</v>
+      </c>
+      <c r="G220" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H220" s="11">
+        <v>2.66</v>
+      </c>
+      <c r="I220" s="11">
+        <v>2.08916</v>
+      </c>
       <c r="J220" s="4"/>
     </row>
     <row r="221" ht="14.25" customHeight="1">
+      <c r="A221" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B221" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C221" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D221" s="2">
+        <v>2050.0</v>
+      </c>
+      <c r="E221" s="11">
+        <v>10.25697219</v>
+      </c>
+      <c r="F221" s="11">
+        <v>1.511411236</v>
+      </c>
+      <c r="G221" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H221" s="11">
+        <v>2.52</v>
+      </c>
+      <c r="I221" s="11">
+        <v>0.55273</v>
+      </c>
       <c r="J221" s="4"/>
     </row>
     <row r="222" ht="14.25" customHeight="1">
@@ -7115,9 +9534,6 @@
     </row>
     <row r="966" ht="14.25" customHeight="1">
       <c r="J966" s="4"/>
-    </row>
-    <row r="967" ht="14.25" customHeight="1">
-      <c r="J967" s="4"/>
     </row>
   </sheetData>
   <printOptions/>
@@ -7128,6 +9544,51 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <pageSetUpPr/>
@@ -7163,7 +9624,7 @@
         <v>12</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>8</v>
@@ -7370,23 +9831,23 @@
     </row>
     <row r="14" ht="14.25" customHeight="1">
       <c r="A14" s="2"/>
-      <c r="B14" s="10"/>
+      <c r="B14" s="13"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
       <c r="F14" s="4"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="2"/>
-      <c r="B15" s="10"/>
-      <c r="E15" s="11"/>
+      <c r="B15" s="13"/>
+      <c r="E15" s="14"/>
       <c r="F15" s="4"/>
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="11"/>
+      <c r="E16" s="14"/>
       <c r="F16" s="4"/>
     </row>
     <row r="17" ht="14.25" customHeight="1">
@@ -7400,7 +9861,7 @@
         <v>12</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>8</v>
@@ -7606,20 +10067,20 @@
       <c r="F28" s="4"/>
     </row>
     <row r="29" ht="14.25" customHeight="1">
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
       <c r="F29" s="4"/>
     </row>
     <row r="30" ht="14.25" customHeight="1">
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
       <c r="F30" s="4"/>
     </row>
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E31" s="11"/>
+      <c r="E31" s="14"/>
       <c r="F31" s="4"/>
     </row>
     <row r="32" ht="14.25" customHeight="1">
@@ -7633,7 +10094,7 @@
         <v>12</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>8</v>
@@ -7848,7 +10309,7 @@
       <c r="A46" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E46" s="11"/>
+      <c r="E46" s="14"/>
       <c r="F46" s="4"/>
     </row>
     <row r="47" ht="14.25" customHeight="1">
@@ -7862,7 +10323,7 @@
         <v>12</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>8</v>
@@ -10901,7 +13362,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <pageSetUpPr/>
@@ -10930,16 +13391,16 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F2" s="4"/>
     </row>
@@ -11161,16 +13622,16 @@
         <v>3</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F17" s="4"/>
     </row>
@@ -11394,16 +13855,16 @@
         <v>3</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F32" s="4"/>
     </row>
@@ -11622,16 +14083,16 @@
         <v>3</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F47" s="4"/>
     </row>

</xml_diff>